<commit_message>
excel automation is completed in calculator project
</commit_message>
<xml_diff>
--- a/Durvesh/Week1Calculator/Data/Input/input.xlsx
+++ b/Durvesh/Week1Calculator/Data/Input/input.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\vajrang\Week1Calculator_Reframework\Data\Input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8872B9-BC25-43BC-97D1-BC1AE163CD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>first</t>
   </si>
@@ -43,13 +37,40 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4	
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -175,7 +199,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -352,23 +376,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,8 +402,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30">
       <c r="A2">
         <v>1</v>
       </c>
@@ -389,8 +416,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30">
       <c r="A3">
         <v>2</v>
       </c>
@@ -400,8 +430,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30">
       <c r="A4">
         <v>3</v>
       </c>
@@ -411,8 +444,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
       <c r="A5">
         <v>4</v>
       </c>
@@ -422,8 +458,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
       <c r="A6">
         <v>5</v>
       </c>
@@ -433,8 +472,11 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30">
       <c r="A7">
         <v>6</v>
       </c>
@@ -444,10 +486,37 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://www.youtube.com/watch?v=4bTTO_ie58o&amp;list=PLFd2UxUMjZNfUqyCCB_zs0cI-7nEO4T8E" xr:uid="{812E8542-1EE5-40F4-A1C6-69F699F45AA0}"/>
+    <hyperlink ref="C4" r:id="rId1" display="https://www.youtube.com/watch?v=4bTTO_ie58o&amp;list=PLFd2UxUMjZNfUqyCCB_zs0cI-7nEO4T8E"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>